<commit_message>
:rocket: Q Learning done
</commit_message>
<xml_diff>
--- a/mlb_batting_stats_cleaned.xlsx
+++ b/mlb_batting_stats_cleaned.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Morillo\Desktop\PythonForML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7404ED1-3679-48CC-8F5A-B6E047569D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAB6025-C2F5-4339-84F7-68325349432C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Estadisticas 2024" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t>jugador</t>
   </si>
@@ -209,13 +222,19 @@
   </si>
   <si>
     <t>Jackson Merrill</t>
+  </si>
+  <si>
+    <t>Babip</t>
+  </si>
+  <si>
+    <t>ISO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,16 +248,30 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -261,20 +294,459 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -285,6 +757,32 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{615D676D-097F-47D8-BF2C-03BA109C4390}" name="Table1" displayName="Table1" ref="A1:O26" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+  <autoFilter ref="A1:O26" xr:uid="{615D676D-097F-47D8-BF2C-03BA109C4390}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{C498E52F-1479-44BB-B8E4-79BA50235EFC}" name="jugador" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{F39E987E-2B19-4E39-8A8A-62760C5E7293}" name="rol" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{F6F0775E-5A27-42C3-82E3-92CCFFC06460}" name="equipo" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{B174F317-3E34-4B6A-9E73-C300876749CC}" name="juegos" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{5CC8BBD7-B283-49B9-973F-FF302F451632}" name="turnos_bateo" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{CBF8770A-FD5D-4B0D-9279-9DAE5040BEB5}" name="hits" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{27B96AB9-89A3-4592-A926-133BC92BB2ED}" name="carreras" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{CD98B2EC-3730-4029-816D-BD52E5618EFC}" name="carreras_impulsadas" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{808B382A-15FB-4315-AB8A-352EF61B97A1}" name="home_runs" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{9B75C48F-1F2D-4527-8436-139AADDB71B8}" name="average" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{E334D84D-1929-4610-B575-8D58DCD94038}" name="obp" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{9089A2DB-B15F-4469-B858-825F8A81A1C7}" name="slg" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{D2380D02-85BF-43A1-861F-348C918FD157}" name="ops" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{2864638B-0793-4B95-9BF9-2E96B4F81777}" name="Babip" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{B2D06FAB-491A-4E2D-84D4-19A6B6690517}" name="ISO" dataDxfId="1">
+      <calculatedColumnFormula>L2-J2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -572,1085 +1070,1276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
+    <col min="7" max="7" width="9.6328125" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="10" max="10" width="9.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="N1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>142</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>564</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>190</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>118</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>97</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>30</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>0.33700000000000002</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="1">
         <v>0.39</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>0.60599999999999998</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <v>0.996</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="N2" s="1">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="O2" s="3">
+        <f>L2-J2</f>
+        <v>0.26899999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>139</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>538</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>176</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>85</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>93</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>28</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>0.32700000000000001</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
         <v>0.39900000000000002</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>0.56100000000000005</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="N3" s="1">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="O3" s="3">
+        <f>L3-J3</f>
+        <v>0.23400000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>140</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>499</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>160</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>109</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>125</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <v>51</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <v>0.32100000000000001</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="1">
         <v>0.45400000000000001</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="1">
         <v>0.69699999999999995</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="1">
         <v>1.151</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="N4" s="1">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="O4" s="3">
+        <f>L4-J4</f>
+        <v>0.37599999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>133</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>498</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>156</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>80</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>80</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <v>32</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="1">
         <v>0.313</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="1">
         <v>0.39800000000000002</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1">
         <v>0.57599999999999996</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="1">
         <v>0.97399999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="N5" s="1">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="O5" s="3">
+        <f>L5-J5</f>
+        <v>0.26299999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>133</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>564</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>175</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>73</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>41</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>4</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>0.31</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="1">
         <v>0.34499999999999997</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="1">
         <v>0.38300000000000001</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="1">
         <v>0.72799999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="N6" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="O6" s="3">
+        <f>L6-J6</f>
+        <v>7.3000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>141</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>531</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>164</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>86</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <v>98</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <v>37</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <v>0.309</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="1">
         <v>0.38200000000000001</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="1">
         <v>0.57099999999999995</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="1">
         <v>0.95299999999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="N7" s="1">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="O7" s="3">
+        <f>L7-J7</f>
+        <v>0.26199999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>126</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>469</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>141</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>74</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>99</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <v>35</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <v>0.30099999999999999</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="1">
         <v>0.372</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="1">
         <v>0.58599999999999997</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="1">
         <v>0.95799999999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="N8" s="1">
+        <v>0.371</v>
+      </c>
+      <c r="O8" s="3">
+        <f>L8-J8</f>
+        <v>0.28499999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>138</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>563</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>169</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>85</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>59</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <v>19</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="1">
         <v>0.3</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="1">
         <v>0.35499999999999998</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="1">
         <v>0.44800000000000001</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="1">
         <v>0.80300000000000005</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="N9" s="1">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="O9" s="3">
+        <f>L9-J9</f>
+        <v>0.14800000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>101</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>424</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>126</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>76</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <v>51</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1">
         <v>16</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>0.29699999999999999</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="1">
         <v>0.34399999999999997</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="1">
         <v>0.46200000000000002</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="1">
         <v>0.80600000000000005</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="N10" s="1">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="O10" s="3">
+        <f>L10-J10</f>
+        <v>0.16500000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>130</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>507</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>150</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>63</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>79</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>16</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>0.29599999999999999</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="1">
         <v>0.32300000000000001</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="1">
         <v>0.44800000000000001</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="1">
         <v>0.77100000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="N11" s="1">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="O11" s="3">
+        <f>L11-J11</f>
+        <v>0.15200000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>138</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>511</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>150</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>113</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="1">
         <v>98</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="1">
         <v>38</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="1">
         <v>0.29399999999999998</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="1">
         <v>0.42199999999999999</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="1">
         <v>0.58699999999999997</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="1">
         <v>1.0089999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="N12" s="1">
+        <v>2.96</v>
+      </c>
+      <c r="O12" s="3">
+        <f>L12-J12</f>
+        <v>0.29299999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>118</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>443</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>130</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>81</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="1">
         <v>81</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="1">
         <v>30</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="1">
         <v>0.29299999999999998</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="1">
         <v>0.36699999999999999</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="1">
         <v>0.55100000000000005</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="1">
         <v>0.91800000000000004</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="N13" s="1">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="O13" s="3">
+        <f>L13-J13</f>
+        <v>0.25800000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>139</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>582</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>170</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>98</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="1">
         <v>72</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="1">
         <v>21</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="1">
         <v>0.29199999999999998</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="1">
         <v>0.35099999999999998</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="1">
         <v>0.52100000000000002</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="1">
         <v>0.872</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="N14" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="O14" s="3">
+        <f>L14-J14</f>
+        <v>0.22900000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>138</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>549</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>160</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>112</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="1">
         <v>100</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="1">
         <v>45</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="1">
         <v>0.29099999999999998</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="1">
         <v>0.376</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="1">
         <v>0.61699999999999999</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="1">
         <v>0.99299999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="N15" s="1">
+        <v>0.314</v>
+      </c>
+      <c r="O15" s="3">
+        <f>L15-J15</f>
+        <v>0.32600000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>138</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>493</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>143</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>70</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="1">
         <v>82</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="1">
         <v>22</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="1">
         <v>0.32100000000000001</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="1">
         <v>0.495</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="1">
         <v>0.81599999999999995</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="N16" s="1">
+        <v>0.316</v>
+      </c>
+      <c r="O16" s="3">
+        <f>L16-J16</f>
+        <v>0.20500000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>131</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>507</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>147</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>59</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="1">
         <v>89</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="1">
         <v>13</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="1">
         <v>0.34300000000000003</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="1">
         <v>0.46200000000000002</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="1">
         <v>0.80500000000000005</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="N17" s="1">
+        <v>0.316</v>
+      </c>
+      <c r="O17" s="3">
+        <f>L17-J17</f>
+        <v>0.17200000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>115</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>459</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>133</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>76</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="1">
         <v>43</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="1">
         <v>13</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="1">
         <v>0.35599999999999998</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="1">
         <v>0.42299999999999999</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="1">
         <v>0.77900000000000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="N18" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="O18" s="3">
+        <f>L18-J18</f>
+        <v>0.13300000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>124</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>442</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>128</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>51</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="1">
         <v>63</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="1">
         <v>15</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="1">
         <v>0.32800000000000001</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="1">
         <v>0.45200000000000001</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="1">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="N19" s="1">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="O19" s="3">
+        <f>L19-J19</f>
+        <v>0.16200000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>129</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>476</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>137</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>74</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="1">
         <v>83</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="1">
         <v>21</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="1">
         <v>0.28799999999999998</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="1">
         <v>0.38300000000000001</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="1">
         <v>0.49399999999999999</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="1">
         <v>0.877</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="N20" s="1">
+        <v>0.312</v>
+      </c>
+      <c r="O20" s="3">
+        <f>L20-J20</f>
+        <v>0.20600000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>126</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>480</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>136</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>75</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="1">
         <v>78</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="1">
         <v>26</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="1">
         <v>0.28299999999999997</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="1">
         <v>0.372</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="1">
         <v>0.51900000000000002</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="1">
         <v>0.89100000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="N21" s="1">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="O21" s="3">
+        <f>L21-J21</f>
+        <v>0.23600000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>141</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>558</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>156</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <v>108</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="1">
         <v>85</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="1">
         <v>36</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="1">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="1">
         <v>0.36499999999999999</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="1">
         <v>0.53900000000000003</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="1">
         <v>0.90400000000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="N22" s="1">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="O22" s="3">
+        <f>L22-J22</f>
+        <v>0.25900000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>125</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>480</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>134</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
         <v>81</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="1">
         <v>81</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="1">
         <v>28</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="1">
         <v>0.27900000000000003</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="1">
         <v>0.35499999999999998</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="1">
         <v>0.54400000000000004</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="1">
         <v>0.89900000000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="N23" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="O23" s="3">
+        <f>L23-J23</f>
+        <v>0.26500000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>130</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>516</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>144</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
         <v>51</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="1">
         <v>64</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="1">
         <v>14</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="1">
         <v>0.27900000000000003</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="1">
         <v>0.33700000000000002</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="1">
         <v>0.41699999999999998</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="1">
         <v>0.754</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="N24" s="1">
+        <v>0.312</v>
+      </c>
+      <c r="O24" s="3">
+        <f>L24-J24</f>
+        <v>0.13799999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>140</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>496</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>138</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <v>80</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="1">
         <v>82</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="1">
         <v>22</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="1">
         <v>0.27800000000000002</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="1">
         <v>0.38200000000000001</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="1">
         <v>0.46</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="1">
         <v>0.84199999999999997</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="N25" s="1">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="O25" s="3">
+        <f>L25-J25</f>
+        <v>0.182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="9">
         <v>123</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="9">
         <v>475</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="9">
         <v>132</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="9">
         <v>68</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="9">
         <v>74</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="9">
         <v>30</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="9">
         <v>0.27800000000000002</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="9">
         <v>0.35299999999999998</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="9">
         <v>0.51200000000000001</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="9">
         <v>0.86499999999999999</v>
       </c>
+      <c r="N26" s="9">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="O26" s="10">
+        <f>L26-J26</f>
+        <v>0.23399999999999999</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O26">
+    <sortCondition descending="1" ref="J2:J26"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>